<commit_message>
corrected quadratic bit wise
</commit_message>
<xml_diff>
--- a/dataExcel.xlsx
+++ b/dataExcel.xlsx
@@ -9,27 +9,29 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet8" sheetId="8" r:id="rId1"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="9" r:id="rId1"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="data" localSheetId="6">Sheet1!$A$1:$D$11</definedName>
-    <definedName name="data" localSheetId="4">Sheet3!$A$1:$AA$11</definedName>
-    <definedName name="data" localSheetId="2">Sheet5!$A$1:$AA$21</definedName>
-    <definedName name="data" localSheetId="0">Sheet8!$A$1:$AA$51</definedName>
-    <definedName name="data_1" localSheetId="5">Sheet2!$A$1:$AA$11</definedName>
-    <definedName name="data_1" localSheetId="3">Sheet4!$A$1:$AA$21</definedName>
-    <definedName name="data_1" localSheetId="1">Sheet6!$A$1:$AA$21</definedName>
+    <definedName name="data" localSheetId="7">Sheet1!$A$1:$D$11</definedName>
+    <definedName name="data" localSheetId="5">Sheet3!$A$1:$AA$11</definedName>
+    <definedName name="data" localSheetId="3">Sheet5!$A$1:$AA$21</definedName>
+    <definedName name="data" localSheetId="1">Sheet8!$A$1:$AA$51</definedName>
+    <definedName name="data_1" localSheetId="6">Sheet2!$A$1:$AA$11</definedName>
+    <definedName name="data_1" localSheetId="4">Sheet4!$A$1:$AA$21</definedName>
+    <definedName name="data_1" localSheetId="2">Sheet6!$A$1:$AA$21</definedName>
+    <definedName name="data_1" localSheetId="0">Sheet7!$A$1:$AA$51</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -44,7 +46,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="data" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" delimited="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" delimited="0" comma="1">
       <textFields count="4">
         <textField/>
         <textField position="3"/>
@@ -54,7 +56,7 @@
     </textPr>
   </connection>
   <connection id="2" name="data1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -64,7 +66,7 @@
     </textPr>
   </connection>
   <connection id="3" name="data2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -72,7 +74,7 @@
     </textPr>
   </connection>
   <connection id="4" name="data3" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -82,14 +84,14 @@
     </textPr>
   </connection>
   <connection id="5" name="data4" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="6" name="data5" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -99,9 +101,18 @@
     </textPr>
   </connection>
   <connection id="7" name="data6" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
       <textFields count="4">
         <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="data7" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lizziechen/Desktop/cs375/finalproject/CS375-Final-Project/data.csv" comma="1">
+      <textFields count="3">
         <textField/>
         <textField/>
         <textField/>
@@ -112,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="62">
   <si>
     <t>line</t>
   </si>
@@ -351,30 +362,34 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -641,9 +656,4282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q33" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>110</v>
+      </c>
+      <c r="T2">
+        <v>76</v>
+      </c>
+      <c r="U2">
+        <v>107</v>
+      </c>
+      <c r="V2">
+        <v>48</v>
+      </c>
+      <c r="W2">
+        <v>32</v>
+      </c>
+      <c r="X2">
+        <v>30</v>
+      </c>
+      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="Z2">
+        <v>8</v>
+      </c>
+      <c r="AA2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>119</v>
+      </c>
+      <c r="T3">
+        <v>86</v>
+      </c>
+      <c r="U3">
+        <v>112</v>
+      </c>
+      <c r="V3">
+        <v>28</v>
+      </c>
+      <c r="W3">
+        <v>26</v>
+      </c>
+      <c r="X3">
+        <v>33</v>
+      </c>
+      <c r="Y3">
+        <v>9</v>
+      </c>
+      <c r="Z3">
+        <v>9</v>
+      </c>
+      <c r="AA3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>127</v>
+      </c>
+      <c r="T4">
+        <v>72</v>
+      </c>
+      <c r="U4">
+        <v>110</v>
+      </c>
+      <c r="V4">
+        <v>30</v>
+      </c>
+      <c r="W4">
+        <v>33</v>
+      </c>
+      <c r="X4">
+        <v>68</v>
+      </c>
+      <c r="Y4">
+        <v>25</v>
+      </c>
+      <c r="Z4">
+        <v>25</v>
+      </c>
+      <c r="AA4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>21</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>101</v>
+      </c>
+      <c r="T5">
+        <v>63</v>
+      </c>
+      <c r="U5">
+        <v>82</v>
+      </c>
+      <c r="V5">
+        <v>38</v>
+      </c>
+      <c r="W5">
+        <v>38</v>
+      </c>
+      <c r="X5">
+        <v>44</v>
+      </c>
+      <c r="Y5">
+        <v>7</v>
+      </c>
+      <c r="Z5">
+        <v>8</v>
+      </c>
+      <c r="AA5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>9</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>77</v>
+      </c>
+      <c r="T6">
+        <v>73</v>
+      </c>
+      <c r="U6">
+        <v>58</v>
+      </c>
+      <c r="V6">
+        <v>111</v>
+      </c>
+      <c r="W6">
+        <v>60</v>
+      </c>
+      <c r="X6">
+        <v>42</v>
+      </c>
+      <c r="Y6">
+        <v>21</v>
+      </c>
+      <c r="Z6">
+        <v>15</v>
+      </c>
+      <c r="AA6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>86</v>
+      </c>
+      <c r="T7">
+        <v>56</v>
+      </c>
+      <c r="U7">
+        <v>72</v>
+      </c>
+      <c r="V7">
+        <v>72</v>
+      </c>
+      <c r="W7">
+        <v>36</v>
+      </c>
+      <c r="X7">
+        <v>20</v>
+      </c>
+      <c r="Y7">
+        <v>10</v>
+      </c>
+      <c r="Z7">
+        <v>10</v>
+      </c>
+      <c r="AA7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>91</v>
+      </c>
+      <c r="T8">
+        <v>71</v>
+      </c>
+      <c r="U8">
+        <v>83</v>
+      </c>
+      <c r="V8">
+        <v>39</v>
+      </c>
+      <c r="W8">
+        <v>35</v>
+      </c>
+      <c r="X8">
+        <v>53</v>
+      </c>
+      <c r="Y8">
+        <v>13</v>
+      </c>
+      <c r="Z8">
+        <v>13</v>
+      </c>
+      <c r="AA8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>59</v>
+      </c>
+      <c r="T9">
+        <v>67</v>
+      </c>
+      <c r="U9">
+        <v>72</v>
+      </c>
+      <c r="V9">
+        <v>51</v>
+      </c>
+      <c r="W9">
+        <v>36</v>
+      </c>
+      <c r="X9">
+        <v>46</v>
+      </c>
+      <c r="Y9">
+        <v>22</v>
+      </c>
+      <c r="Z9">
+        <v>18</v>
+      </c>
+      <c r="AA9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>143</v>
+      </c>
+      <c r="T10">
+        <v>87</v>
+      </c>
+      <c r="U10">
+        <v>101</v>
+      </c>
+      <c r="V10">
+        <v>25</v>
+      </c>
+      <c r="W10">
+        <v>28</v>
+      </c>
+      <c r="X10">
+        <v>46</v>
+      </c>
+      <c r="Y10">
+        <v>13</v>
+      </c>
+      <c r="Z10">
+        <v>11</v>
+      </c>
+      <c r="AA10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>68</v>
+      </c>
+      <c r="T11">
+        <v>58</v>
+      </c>
+      <c r="U11">
+        <v>104</v>
+      </c>
+      <c r="V11">
+        <v>55</v>
+      </c>
+      <c r="W11">
+        <v>47</v>
+      </c>
+      <c r="X11">
+        <v>42</v>
+      </c>
+      <c r="Y11">
+        <v>14</v>
+      </c>
+      <c r="Z11">
+        <v>20</v>
+      </c>
+      <c r="AA11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>96</v>
+      </c>
+      <c r="T12">
+        <v>70</v>
+      </c>
+      <c r="U12">
+        <v>100</v>
+      </c>
+      <c r="V12">
+        <v>32</v>
+      </c>
+      <c r="W12">
+        <v>34</v>
+      </c>
+      <c r="X12">
+        <v>42</v>
+      </c>
+      <c r="Y12">
+        <v>21</v>
+      </c>
+      <c r="Z12">
+        <v>16</v>
+      </c>
+      <c r="AA12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>87</v>
+      </c>
+      <c r="T13">
+        <v>62</v>
+      </c>
+      <c r="U13">
+        <v>100</v>
+      </c>
+      <c r="V13">
+        <v>42</v>
+      </c>
+      <c r="W13">
+        <v>33</v>
+      </c>
+      <c r="X13">
+        <v>35</v>
+      </c>
+      <c r="Y13">
+        <v>11</v>
+      </c>
+      <c r="Z13">
+        <v>8</v>
+      </c>
+      <c r="AA13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>232</v>
+      </c>
+      <c r="T14">
+        <v>122</v>
+      </c>
+      <c r="U14">
+        <v>129</v>
+      </c>
+      <c r="V14">
+        <v>31</v>
+      </c>
+      <c r="W14">
+        <v>25</v>
+      </c>
+      <c r="X14">
+        <v>38</v>
+      </c>
+      <c r="Y14">
+        <v>19</v>
+      </c>
+      <c r="Z14">
+        <v>20</v>
+      </c>
+      <c r="AA14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>11</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>150</v>
+      </c>
+      <c r="T15">
+        <v>106</v>
+      </c>
+      <c r="U15">
+        <v>102</v>
+      </c>
+      <c r="V15">
+        <v>26</v>
+      </c>
+      <c r="W15">
+        <v>27</v>
+      </c>
+      <c r="X15">
+        <v>37</v>
+      </c>
+      <c r="Y15">
+        <v>19</v>
+      </c>
+      <c r="Z15">
+        <v>15</v>
+      </c>
+      <c r="AA15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>9</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>8</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>80</v>
+      </c>
+      <c r="T16">
+        <v>58</v>
+      </c>
+      <c r="U16">
+        <v>101</v>
+      </c>
+      <c r="V16">
+        <v>31</v>
+      </c>
+      <c r="W16">
+        <v>36</v>
+      </c>
+      <c r="X16">
+        <v>43</v>
+      </c>
+      <c r="Y16">
+        <v>10</v>
+      </c>
+      <c r="Z16">
+        <v>11</v>
+      </c>
+      <c r="AA16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>18</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>83</v>
+      </c>
+      <c r="T17">
+        <v>77</v>
+      </c>
+      <c r="U17">
+        <v>116</v>
+      </c>
+      <c r="V17">
+        <v>33</v>
+      </c>
+      <c r="W17">
+        <v>29</v>
+      </c>
+      <c r="X17">
+        <v>32</v>
+      </c>
+      <c r="Y17">
+        <v>5</v>
+      </c>
+      <c r="Z17">
+        <v>5</v>
+      </c>
+      <c r="AA17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>66</v>
+      </c>
+      <c r="T18">
+        <v>44</v>
+      </c>
+      <c r="U18">
+        <v>67</v>
+      </c>
+      <c r="V18">
+        <v>30</v>
+      </c>
+      <c r="W18">
+        <v>25</v>
+      </c>
+      <c r="X18">
+        <v>34</v>
+      </c>
+      <c r="Y18">
+        <v>9</v>
+      </c>
+      <c r="Z18">
+        <v>8</v>
+      </c>
+      <c r="AA18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>58</v>
+      </c>
+      <c r="B19">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>100</v>
+      </c>
+      <c r="T19">
+        <v>82</v>
+      </c>
+      <c r="U19">
+        <v>111</v>
+      </c>
+      <c r="V19">
+        <v>37</v>
+      </c>
+      <c r="W19">
+        <v>33</v>
+      </c>
+      <c r="X19">
+        <v>33</v>
+      </c>
+      <c r="Y19">
+        <v>17</v>
+      </c>
+      <c r="Z19">
+        <v>14</v>
+      </c>
+      <c r="AA19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>14</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>87</v>
+      </c>
+      <c r="T20">
+        <v>68</v>
+      </c>
+      <c r="U20">
+        <v>76</v>
+      </c>
+      <c r="V20">
+        <v>57</v>
+      </c>
+      <c r="W20">
+        <v>37</v>
+      </c>
+      <c r="X20">
+        <v>44</v>
+      </c>
+      <c r="Y20">
+        <v>13</v>
+      </c>
+      <c r="Z20">
+        <v>10</v>
+      </c>
+      <c r="AA20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>15</v>
+      </c>
+      <c r="L21">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>124</v>
+      </c>
+      <c r="T21">
+        <v>94</v>
+      </c>
+      <c r="U21">
+        <v>97</v>
+      </c>
+      <c r="V21">
+        <v>66</v>
+      </c>
+      <c r="W21">
+        <v>35</v>
+      </c>
+      <c r="X21">
+        <v>32</v>
+      </c>
+      <c r="Y21">
+        <v>12</v>
+      </c>
+      <c r="Z21">
+        <v>12</v>
+      </c>
+      <c r="AA21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>146</v>
+      </c>
+      <c r="T22">
+        <v>94</v>
+      </c>
+      <c r="U22">
+        <v>114</v>
+      </c>
+      <c r="V22">
+        <v>40</v>
+      </c>
+      <c r="W22">
+        <v>33</v>
+      </c>
+      <c r="X22">
+        <v>37</v>
+      </c>
+      <c r="Y22">
+        <v>15</v>
+      </c>
+      <c r="Z22">
+        <v>22</v>
+      </c>
+      <c r="AA22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>13</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>167</v>
+      </c>
+      <c r="T23">
+        <v>95</v>
+      </c>
+      <c r="U23">
+        <v>120</v>
+      </c>
+      <c r="V23">
+        <v>23</v>
+      </c>
+      <c r="W23">
+        <v>30</v>
+      </c>
+      <c r="X23">
+        <v>33</v>
+      </c>
+      <c r="Y23">
+        <v>8</v>
+      </c>
+      <c r="Z23">
+        <v>8</v>
+      </c>
+      <c r="AA23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>100</v>
+      </c>
+      <c r="T24">
+        <v>76</v>
+      </c>
+      <c r="U24">
+        <v>118</v>
+      </c>
+      <c r="V24">
+        <v>27</v>
+      </c>
+      <c r="W24">
+        <v>26</v>
+      </c>
+      <c r="X24">
+        <v>34</v>
+      </c>
+      <c r="Y24">
+        <v>20</v>
+      </c>
+      <c r="Z24">
+        <v>14</v>
+      </c>
+      <c r="AA24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>17</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>7</v>
+      </c>
+      <c r="K25">
+        <v>15</v>
+      </c>
+      <c r="L25">
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>75</v>
+      </c>
+      <c r="T25">
+        <v>74</v>
+      </c>
+      <c r="U25">
+        <v>88</v>
+      </c>
+      <c r="V25">
+        <v>42</v>
+      </c>
+      <c r="W25">
+        <v>30</v>
+      </c>
+      <c r="X25">
+        <v>47</v>
+      </c>
+      <c r="Y25">
+        <v>11</v>
+      </c>
+      <c r="Z25">
+        <v>11</v>
+      </c>
+      <c r="AA25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>98</v>
+      </c>
+      <c r="T26">
+        <v>64</v>
+      </c>
+      <c r="U26">
+        <v>117</v>
+      </c>
+      <c r="V26">
+        <v>46</v>
+      </c>
+      <c r="W26">
+        <v>48</v>
+      </c>
+      <c r="X26">
+        <v>47</v>
+      </c>
+      <c r="Y26">
+        <v>10</v>
+      </c>
+      <c r="Z26">
+        <v>11</v>
+      </c>
+      <c r="AA26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <v>5</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>60</v>
+      </c>
+      <c r="T27">
+        <v>48</v>
+      </c>
+      <c r="U27">
+        <v>72</v>
+      </c>
+      <c r="V27">
+        <v>50</v>
+      </c>
+      <c r="W27">
+        <v>39</v>
+      </c>
+      <c r="X27">
+        <v>41</v>
+      </c>
+      <c r="Y27">
+        <v>16</v>
+      </c>
+      <c r="Z27">
+        <v>14</v>
+      </c>
+      <c r="AA27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="N28">
+        <v>4</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>125</v>
+      </c>
+      <c r="T28">
+        <v>86</v>
+      </c>
+      <c r="U28">
+        <v>102</v>
+      </c>
+      <c r="V28">
+        <v>47</v>
+      </c>
+      <c r="W28">
+        <v>30</v>
+      </c>
+      <c r="X28">
+        <v>42</v>
+      </c>
+      <c r="Y28">
+        <v>10</v>
+      </c>
+      <c r="Z28">
+        <v>12</v>
+      </c>
+      <c r="AA28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>18</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>15</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>107</v>
+      </c>
+      <c r="T29">
+        <v>118</v>
+      </c>
+      <c r="U29">
+        <v>93</v>
+      </c>
+      <c r="V29">
+        <v>21</v>
+      </c>
+      <c r="W29">
+        <v>24</v>
+      </c>
+      <c r="X29">
+        <v>31</v>
+      </c>
+      <c r="Y29">
+        <v>12</v>
+      </c>
+      <c r="Z29">
+        <v>12</v>
+      </c>
+      <c r="AA29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>33</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>12</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+      <c r="K30">
+        <v>8</v>
+      </c>
+      <c r="L30">
+        <v>18</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>130</v>
+      </c>
+      <c r="T30">
+        <v>104</v>
+      </c>
+      <c r="U30">
+        <v>124</v>
+      </c>
+      <c r="V30">
+        <v>27</v>
+      </c>
+      <c r="W30">
+        <v>38</v>
+      </c>
+      <c r="X30">
+        <v>42</v>
+      </c>
+      <c r="Y30">
+        <v>12</v>
+      </c>
+      <c r="Z30">
+        <v>14</v>
+      </c>
+      <c r="AA30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>13</v>
+      </c>
+      <c r="K31">
+        <v>8</v>
+      </c>
+      <c r="L31">
+        <v>14</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>122</v>
+      </c>
+      <c r="T31">
+        <v>95</v>
+      </c>
+      <c r="U31">
+        <v>79</v>
+      </c>
+      <c r="V31">
+        <v>28</v>
+      </c>
+      <c r="W31">
+        <v>35</v>
+      </c>
+      <c r="X31">
+        <v>44</v>
+      </c>
+      <c r="Y31">
+        <v>16</v>
+      </c>
+      <c r="Z31">
+        <v>14</v>
+      </c>
+      <c r="AA31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>16</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>7</v>
+      </c>
+      <c r="K32">
+        <v>5</v>
+      </c>
+      <c r="L32">
+        <v>6</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>59</v>
+      </c>
+      <c r="T32">
+        <v>62</v>
+      </c>
+      <c r="U32">
+        <v>68</v>
+      </c>
+      <c r="V32">
+        <v>70</v>
+      </c>
+      <c r="W32">
+        <v>41</v>
+      </c>
+      <c r="X32">
+        <v>49</v>
+      </c>
+      <c r="Y32">
+        <v>32</v>
+      </c>
+      <c r="Z32">
+        <v>17</v>
+      </c>
+      <c r="AA32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>18</v>
+      </c>
+      <c r="C33">
+        <v>22</v>
+      </c>
+      <c r="D33">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>11</v>
+      </c>
+      <c r="K33">
+        <v>6</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>6</v>
+      </c>
+      <c r="N33">
+        <v>6</v>
+      </c>
+      <c r="O33">
+        <v>8</v>
+      </c>
+      <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>103</v>
+      </c>
+      <c r="T33">
+        <v>76</v>
+      </c>
+      <c r="U33">
+        <v>92</v>
+      </c>
+      <c r="V33">
+        <v>43</v>
+      </c>
+      <c r="W33">
+        <v>31</v>
+      </c>
+      <c r="X33">
+        <v>26</v>
+      </c>
+      <c r="Y33">
+        <v>12</v>
+      </c>
+      <c r="Z33">
+        <v>12</v>
+      </c>
+      <c r="AA33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>29</v>
+      </c>
+      <c r="D34">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>4</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>81</v>
+      </c>
+      <c r="T34">
+        <v>69</v>
+      </c>
+      <c r="U34">
+        <v>117</v>
+      </c>
+      <c r="V34">
+        <v>47</v>
+      </c>
+      <c r="W34">
+        <v>29</v>
+      </c>
+      <c r="X34">
+        <v>44</v>
+      </c>
+      <c r="Y34">
+        <v>11</v>
+      </c>
+      <c r="Z34">
+        <v>9</v>
+      </c>
+      <c r="AA34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>28</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <v>7</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>101</v>
+      </c>
+      <c r="T35">
+        <v>75</v>
+      </c>
+      <c r="U35">
+        <v>63</v>
+      </c>
+      <c r="V35">
+        <v>71</v>
+      </c>
+      <c r="W35">
+        <v>40</v>
+      </c>
+      <c r="X35">
+        <v>53</v>
+      </c>
+      <c r="Y35">
+        <v>17</v>
+      </c>
+      <c r="Z35">
+        <v>15</v>
+      </c>
+      <c r="AA35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <v>11</v>
+      </c>
+      <c r="K36">
+        <v>7</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>105</v>
+      </c>
+      <c r="T36">
+        <v>93</v>
+      </c>
+      <c r="U36">
+        <v>79</v>
+      </c>
+      <c r="V36">
+        <v>15</v>
+      </c>
+      <c r="W36">
+        <v>25</v>
+      </c>
+      <c r="X36">
+        <v>29</v>
+      </c>
+      <c r="Y36">
+        <v>13</v>
+      </c>
+      <c r="Z36">
+        <v>13</v>
+      </c>
+      <c r="AA36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>56</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>23</v>
+      </c>
+      <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37">
+        <v>14</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>8</v>
+      </c>
+      <c r="K37">
+        <v>8</v>
+      </c>
+      <c r="L37">
+        <v>5</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <v>3</v>
+      </c>
+      <c r="P37">
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <v>94</v>
+      </c>
+      <c r="T37">
+        <v>90</v>
+      </c>
+      <c r="U37">
+        <v>86</v>
+      </c>
+      <c r="V37">
+        <v>60</v>
+      </c>
+      <c r="W37">
+        <v>33</v>
+      </c>
+      <c r="X37">
+        <v>28</v>
+      </c>
+      <c r="Y37">
+        <v>8</v>
+      </c>
+      <c r="Z37">
+        <v>8</v>
+      </c>
+      <c r="AA37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>43</v>
+      </c>
+      <c r="B38">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>24</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="M38">
+        <v>5</v>
+      </c>
+      <c r="N38">
+        <v>6</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <v>99</v>
+      </c>
+      <c r="T38">
+        <v>72</v>
+      </c>
+      <c r="U38">
+        <v>110</v>
+      </c>
+      <c r="V38">
+        <v>26</v>
+      </c>
+      <c r="W38">
+        <v>30</v>
+      </c>
+      <c r="X38">
+        <v>56</v>
+      </c>
+      <c r="Y38">
+        <v>5</v>
+      </c>
+      <c r="Z38">
+        <v>6</v>
+      </c>
+      <c r="AA38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>26</v>
+      </c>
+      <c r="C39">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <v>7</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>2</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39">
+        <v>3</v>
+      </c>
+      <c r="S39">
+        <v>96</v>
+      </c>
+      <c r="T39">
+        <v>90</v>
+      </c>
+      <c r="U39">
+        <v>107</v>
+      </c>
+      <c r="V39">
+        <v>36</v>
+      </c>
+      <c r="W39">
+        <v>36</v>
+      </c>
+      <c r="X39">
+        <v>61</v>
+      </c>
+      <c r="Y39">
+        <v>16</v>
+      </c>
+      <c r="Z39">
+        <v>11</v>
+      </c>
+      <c r="AA39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>33</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>14</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>7</v>
+      </c>
+      <c r="K40">
+        <v>5</v>
+      </c>
+      <c r="L40">
+        <v>5</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>85</v>
+      </c>
+      <c r="T40">
+        <v>68</v>
+      </c>
+      <c r="U40">
+        <v>84</v>
+      </c>
+      <c r="V40">
+        <v>46</v>
+      </c>
+      <c r="W40">
+        <v>42</v>
+      </c>
+      <c r="X40">
+        <v>37</v>
+      </c>
+      <c r="Y40">
+        <v>3</v>
+      </c>
+      <c r="Z40">
+        <v>3</v>
+      </c>
+      <c r="AA40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>26</v>
+      </c>
+      <c r="C41">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>21</v>
+      </c>
+      <c r="E41">
+        <v>18</v>
+      </c>
+      <c r="F41">
+        <v>13</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <v>4</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>250</v>
+      </c>
+      <c r="T41">
+        <v>131</v>
+      </c>
+      <c r="U41">
+        <v>96</v>
+      </c>
+      <c r="V41">
+        <v>35</v>
+      </c>
+      <c r="W41">
+        <v>26</v>
+      </c>
+      <c r="X41">
+        <v>23</v>
+      </c>
+      <c r="Y41">
+        <v>9</v>
+      </c>
+      <c r="Z41">
+        <v>9</v>
+      </c>
+      <c r="AA41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>30</v>
+      </c>
+      <c r="B42">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <v>35</v>
+      </c>
+      <c r="D42">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>13</v>
+      </c>
+      <c r="K42">
+        <v>7</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+      <c r="M42">
+        <v>3</v>
+      </c>
+      <c r="N42">
+        <v>3</v>
+      </c>
+      <c r="O42">
+        <v>5</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>154</v>
+      </c>
+      <c r="T42">
+        <v>99</v>
+      </c>
+      <c r="U42">
+        <v>151</v>
+      </c>
+      <c r="V42">
+        <v>33</v>
+      </c>
+      <c r="W42">
+        <v>19</v>
+      </c>
+      <c r="X42">
+        <v>16</v>
+      </c>
+      <c r="Y42">
+        <v>5</v>
+      </c>
+      <c r="Z42">
+        <v>5</v>
+      </c>
+      <c r="AA42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>28</v>
+      </c>
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>19</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>6</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>2</v>
+      </c>
+      <c r="Q43">
+        <v>3</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>183</v>
+      </c>
+      <c r="T43">
+        <v>79</v>
+      </c>
+      <c r="U43">
+        <v>80</v>
+      </c>
+      <c r="V43">
+        <v>20</v>
+      </c>
+      <c r="W43">
+        <v>19</v>
+      </c>
+      <c r="X43">
+        <v>24</v>
+      </c>
+      <c r="Y43">
+        <v>18</v>
+      </c>
+      <c r="Z43">
+        <v>20</v>
+      </c>
+      <c r="AA43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>12</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>6</v>
+      </c>
+      <c r="K44">
+        <v>6</v>
+      </c>
+      <c r="L44">
+        <v>4</v>
+      </c>
+      <c r="M44">
+        <v>4</v>
+      </c>
+      <c r="N44">
+        <v>6</v>
+      </c>
+      <c r="O44">
+        <v>6</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>62</v>
+      </c>
+      <c r="T44">
+        <v>66</v>
+      </c>
+      <c r="U44">
+        <v>89</v>
+      </c>
+      <c r="V44">
+        <v>24</v>
+      </c>
+      <c r="W44">
+        <v>22</v>
+      </c>
+      <c r="X44">
+        <v>36</v>
+      </c>
+      <c r="Y44">
+        <v>4</v>
+      </c>
+      <c r="Z44">
+        <v>4</v>
+      </c>
+      <c r="AA44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>18</v>
+      </c>
+      <c r="D45">
+        <v>17</v>
+      </c>
+      <c r="E45">
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="K45">
+        <v>7</v>
+      </c>
+      <c r="L45">
+        <v>3</v>
+      </c>
+      <c r="M45">
+        <v>6</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>99</v>
+      </c>
+      <c r="T45">
+        <v>86</v>
+      </c>
+      <c r="U45">
+        <v>100</v>
+      </c>
+      <c r="V45">
+        <v>44</v>
+      </c>
+      <c r="W45">
+        <v>45</v>
+      </c>
+      <c r="X45">
+        <v>45</v>
+      </c>
+      <c r="Y45">
+        <v>12</v>
+      </c>
+      <c r="Z45">
+        <v>12</v>
+      </c>
+      <c r="AA45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>11</v>
+      </c>
+      <c r="F46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>7</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46">
+        <v>2</v>
+      </c>
+      <c r="N46">
+        <v>2</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>3</v>
+      </c>
+      <c r="Q46">
+        <v>3</v>
+      </c>
+      <c r="R46">
+        <v>2</v>
+      </c>
+      <c r="S46">
+        <v>142</v>
+      </c>
+      <c r="T46">
+        <v>90</v>
+      </c>
+      <c r="U46">
+        <v>116</v>
+      </c>
+      <c r="V46">
+        <v>31</v>
+      </c>
+      <c r="W46">
+        <v>36</v>
+      </c>
+      <c r="X46">
+        <v>28</v>
+      </c>
+      <c r="Y46">
+        <v>21</v>
+      </c>
+      <c r="Z46">
+        <v>24</v>
+      </c>
+      <c r="AA46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>30</v>
+      </c>
+      <c r="E47">
+        <v>18</v>
+      </c>
+      <c r="F47">
+        <v>16</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47">
+        <v>5</v>
+      </c>
+      <c r="J47">
+        <v>11</v>
+      </c>
+      <c r="K47">
+        <v>15</v>
+      </c>
+      <c r="L47">
+        <v>7</v>
+      </c>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="N47">
+        <v>6</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+      <c r="P47">
+        <v>3</v>
+      </c>
+      <c r="Q47">
+        <v>3</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <v>135</v>
+      </c>
+      <c r="T47">
+        <v>81</v>
+      </c>
+      <c r="U47">
+        <v>92</v>
+      </c>
+      <c r="V47">
+        <v>19</v>
+      </c>
+      <c r="W47">
+        <v>18</v>
+      </c>
+      <c r="X47">
+        <v>42</v>
+      </c>
+      <c r="Y47">
+        <v>9</v>
+      </c>
+      <c r="Z47">
+        <v>10</v>
+      </c>
+      <c r="AA47">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>17</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>12</v>
+      </c>
+      <c r="K48">
+        <v>9</v>
+      </c>
+      <c r="L48">
+        <v>11</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <v>88</v>
+      </c>
+      <c r="T48">
+        <v>54</v>
+      </c>
+      <c r="U48">
+        <v>85</v>
+      </c>
+      <c r="V48">
+        <v>26</v>
+      </c>
+      <c r="W48">
+        <v>20</v>
+      </c>
+      <c r="X48">
+        <v>38</v>
+      </c>
+      <c r="Y48">
+        <v>10</v>
+      </c>
+      <c r="Z48">
+        <v>9</v>
+      </c>
+      <c r="AA48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>38</v>
+      </c>
+      <c r="B49">
+        <v>27</v>
+      </c>
+      <c r="C49">
+        <v>25</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <v>3</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <v>3</v>
+      </c>
+      <c r="S49">
+        <v>127</v>
+      </c>
+      <c r="T49">
+        <v>83</v>
+      </c>
+      <c r="U49">
+        <v>90</v>
+      </c>
+      <c r="V49">
+        <v>37</v>
+      </c>
+      <c r="W49">
+        <v>42</v>
+      </c>
+      <c r="X49">
+        <v>42</v>
+      </c>
+      <c r="Y49">
+        <v>14</v>
+      </c>
+      <c r="Z49">
+        <v>12</v>
+      </c>
+      <c r="AA49">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>33</v>
+      </c>
+      <c r="B50">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50">
+        <v>6</v>
+      </c>
+      <c r="G50">
+        <v>6</v>
+      </c>
+      <c r="H50">
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <v>11</v>
+      </c>
+      <c r="J50">
+        <v>3</v>
+      </c>
+      <c r="K50">
+        <v>4</v>
+      </c>
+      <c r="L50">
+        <v>10</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>2</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>199</v>
+      </c>
+      <c r="T50">
+        <v>91</v>
+      </c>
+      <c r="U50">
+        <v>76</v>
+      </c>
+      <c r="V50">
+        <v>25</v>
+      </c>
+      <c r="W50">
+        <v>25</v>
+      </c>
+      <c r="X50">
+        <v>36</v>
+      </c>
+      <c r="Y50">
+        <v>7</v>
+      </c>
+      <c r="Z50">
+        <v>7</v>
+      </c>
+      <c r="AA50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+      <c r="D51">
+        <v>18</v>
+      </c>
+      <c r="E51">
+        <v>12</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+      <c r="K51">
+        <v>5</v>
+      </c>
+      <c r="L51">
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <v>3</v>
+      </c>
+      <c r="N51">
+        <v>3</v>
+      </c>
+      <c r="O51">
+        <v>6</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>53</v>
+      </c>
+      <c r="T51">
+        <v>53</v>
+      </c>
+      <c r="U51">
+        <v>103</v>
+      </c>
+      <c r="V51">
+        <v>26</v>
+      </c>
+      <c r="W51">
+        <v>28</v>
+      </c>
+      <c r="X51">
+        <v>29</v>
+      </c>
+      <c r="Y51">
+        <v>15</v>
+      </c>
+      <c r="Z51">
+        <v>11</v>
+      </c>
+      <c r="AA51">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
@@ -5024,7 +9312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA22"/>
   <sheetViews>
@@ -6910,7 +11198,7 @@
         <v>11</v>
       </c>
       <c r="AA22">
-        <f t="shared" ref="B22:AA22" si="1">AVERAGE(AA2:AA21)</f>
+        <f t="shared" ref="AA22" si="1">AVERAGE(AA2:AA21)</f>
         <v>11.75</v>
       </c>
     </row>
@@ -6919,7 +11207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA22"/>
   <sheetViews>
@@ -8814,7 +13102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA26"/>
   <sheetViews>
@@ -10596,111 +14884,111 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>AVERAGE(A2:A21)</f>
+        <f t="shared" ref="A22:AA22" si="0">AVERAGE(A2:A21)</f>
         <v>29.85</v>
       </c>
       <c r="B22">
-        <f>AVERAGE(B2:B21)</f>
+        <f t="shared" si="0"/>
         <v>40.85</v>
       </c>
       <c r="C22">
-        <f>AVERAGE(C2:C21)</f>
+        <f t="shared" si="0"/>
         <v>28.35</v>
       </c>
       <c r="D22">
-        <f>AVERAGE(D2:D21)</f>
+        <f t="shared" si="0"/>
         <v>12.9</v>
       </c>
       <c r="E22">
-        <f>AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>11.1</v>
       </c>
       <c r="F22">
-        <f>AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>10.25</v>
       </c>
       <c r="G22">
-        <f>AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>2.95</v>
       </c>
       <c r="H22">
-        <f>AVERAGE(H2:H21)</f>
+        <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
       <c r="I22">
-        <f>AVERAGE(I2:I21)</f>
+        <f t="shared" si="0"/>
         <v>4.55</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(J2:J21)</f>
+        <f t="shared" si="0"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="K22">
-        <f>AVERAGE(K2:K21)</f>
+        <f t="shared" si="0"/>
         <v>15.55</v>
       </c>
       <c r="L22">
-        <f>AVERAGE(L2:L21)</f>
+        <f t="shared" si="0"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="M22">
-        <f>AVERAGE(M2:M21)</f>
+        <f t="shared" si="0"/>
         <v>3.65</v>
       </c>
       <c r="N22">
-        <f>AVERAGE(N2:N21)</f>
+        <f t="shared" si="0"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="O22">
-        <f>AVERAGE(O2:O21)</f>
+        <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(P2:P21)</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="Q22">
-        <f>AVERAGE(Q2:Q21)</f>
+        <f t="shared" si="0"/>
         <v>2.0499999999999998</v>
       </c>
       <c r="R22">
-        <f>AVERAGE(R2:R21)</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="S22">
-        <f>AVERAGE(S2:S21)</f>
+        <f t="shared" si="0"/>
         <v>123.3</v>
       </c>
       <c r="T22">
-        <f>AVERAGE(T2:T21)</f>
+        <f t="shared" si="0"/>
         <v>155.15</v>
       </c>
       <c r="U22">
-        <f>AVERAGE(U2:U21)</f>
+        <f t="shared" si="0"/>
         <v>201.15</v>
       </c>
       <c r="V22">
-        <f>AVERAGE(V2:V21)</f>
+        <f t="shared" si="0"/>
         <v>46.85</v>
       </c>
       <c r="W22">
-        <f>AVERAGE(W2:W21)</f>
+        <f t="shared" si="0"/>
         <v>38.700000000000003</v>
       </c>
       <c r="X22">
-        <f>AVERAGE(X2:X21)</f>
+        <f t="shared" si="0"/>
         <v>66.099999999999994</v>
       </c>
       <c r="Y22">
-        <f>AVERAGE(Y2:Y21)</f>
+        <f t="shared" si="0"/>
         <v>12.75</v>
       </c>
       <c r="Z22">
-        <f>AVERAGE(Z2:Z21)</f>
+        <f t="shared" si="0"/>
         <v>12.75</v>
       </c>
       <c r="AA22">
-        <f>AVERAGE(AA2:AA21)</f>
+        <f t="shared" si="0"/>
         <v>17.55</v>
       </c>
     </row>
@@ -10718,27 +15006,27 @@
         <v>0.9</v>
       </c>
       <c r="D25">
-        <f>G22</f>
+        <f t="shared" ref="D25:F26" si="1">G22</f>
         <v>2.95</v>
       </c>
       <c r="E25">
-        <f>H22</f>
+        <f t="shared" si="1"/>
         <v>3.3</v>
       </c>
       <c r="F25">
-        <f>I22</f>
+        <f t="shared" si="1"/>
         <v>4.55</v>
       </c>
       <c r="G25">
-        <f>Y22</f>
+        <f t="shared" ref="G25:I26" si="2">Y22</f>
         <v>12.75</v>
       </c>
       <c r="H25">
-        <f>Z22</f>
+        <f t="shared" si="2"/>
         <v>12.75</v>
       </c>
       <c r="I25">
-        <f>AA22</f>
+        <f t="shared" si="2"/>
         <v>17.55</v>
       </c>
     </row>
@@ -10756,27 +15044,27 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <f>G23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E26">
-        <f>H23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>I23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G26">
-        <f>Y23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H26">
-        <f>Z23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I26">
-        <f>AA23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10785,7 +15073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA11"/>
   <sheetViews>
@@ -11740,7 +16028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA11"/>
   <sheetViews>
@@ -12690,7 +16978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>

</xml_diff>